<commit_message>
a push so zip matches 4-mill folder
found a bad error, all fixed now
</commit_message>
<xml_diff>
--- a/4-mill-vent/BOM.xlsx
+++ b/4-mill-vent/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dogma\OneDrive\Desktop\1-mill\4-mill-vent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F579FA-7720-497C-B9F2-2F64BE542AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A618C191-504A-4A8F-919A-9D8C658E45D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="2280" windowWidth="18108" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="E73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>